<commit_message>
Trained Gemma 3 on 50 examples
</commit_message>
<xml_diff>
--- a/results/Semantic_Similarities_Gemma_untrained.xlsx
+++ b/results/Semantic_Similarities_Gemma_untrained.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6462521553039551</v>
+        <v>0.6920520663261414</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6628837585449219</v>
+        <v>0.729717493057251</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6068467497825623</v>
+        <v>0.6769880056381226</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5580381155014038</v>
+        <v>0.3804360330104828</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.5107558965682983</v>
+        <v>0.4451932609081268</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.564617395401001</v>
+        <v>0.5703897476196289</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.4366930723190308</v>
+        <v>0.5163048505783081</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.3366317749023438</v>
+        <v>0.5279713273048401</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6024672985076904</v>
+        <v>0.6451247334480286</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.6060081124305725</v>
+        <v>0.5678476691246033</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5424911975860596</v>
+        <v>0.7257301807403564</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.3611407279968262</v>
+        <v>0.4742555022239685</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.623456597328186</v>
+        <v>0.5271262526512146</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5147656202316284</v>
+        <v>0.4080379903316498</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.6677517294883728</v>
+        <v>0.4415383338928223</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2951507568359375</v>
+        <v>0.5665831565856934</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5056720972061157</v>
+        <v>0.3711598515510559</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.5602142810821533</v>
+        <v>0.2795150279998779</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.4136511981487274</v>
+        <v>0.5485844612121582</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5593957901000977</v>
+        <v>0.5284099578857422</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.6494208574295044</v>
+        <v>0.3018908202648163</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.5000379085540771</v>
+        <v>0.4606550931930542</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5394431352615356</v>
+        <v>0.6264884471893311</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2365057915449142</v>
+        <v>0.6407639384269714</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.6105104684829712</v>
+        <v>0.6765548586845398</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.4436776041984558</v>
+        <v>0.5343475341796875</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.5244687795639038</v>
+        <v>0.5300296545028687</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.5797606110572815</v>
+        <v>0.3813424110412598</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.5820255279541016</v>
+        <v>0.7179755568504333</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.6251950263977051</v>
+        <v>0.4929227530956268</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.476477712392807</v>
+        <v>0.4931705892086029</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.4765832424163818</v>
+        <v>0.465474009513855</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.6421545743942261</v>
+        <v>0.6304359436035156</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.3913838565349579</v>
+        <v>0.5595799684524536</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.3056257665157318</v>
+        <v>0.5026155710220337</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3664053082466125</v>
+        <v>0.3131013512611389</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.5999048352241516</v>
+        <v>0.62077397108078</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.5159176588058472</v>
+        <v>0.689457893371582</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5605567097663879</v>
+        <v>0.5764554738998413</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.7372422218322754</v>
+        <v>0.6119536161422729</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.3964878916740417</v>
+        <v>0.3172469437122345</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.3243905007839203</v>
+        <v>0.3223828971385956</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.422117292881012</v>
+        <v>0.3950381875038147</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.2862460613250732</v>
+        <v>0.4986931681632996</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.3894328474998474</v>
+        <v>0.5837039947509766</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.2970485687255859</v>
+        <v>0.6700018644332886</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.4039145708084106</v>
+        <v>0.4231172204017639</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.5246758460998535</v>
+        <v>0.4077571332454681</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.2432638108730316</v>
+        <v>0.3140339255332947</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.3493852019309998</v>
+        <v>0.608534574508667</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.4736778438091278</v>
+        <v>0.3757619857788086</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.5475079417228699</v>
+        <v>0.3638131022453308</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.2269750535488129</v>
+        <v>0.464464008808136</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.7174538373947144</v>
+        <v>0.4007188677787781</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.6495885848999023</v>
+        <v>0.5289671421051025</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.4163876473903656</v>
+        <v>0.4455665647983551</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.5600242614746094</v>
+        <v>0.4342573285102844</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.6737767457962036</v>
+        <v>0.5671559572219849</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.4482112526893616</v>
+        <v>0.5466420650482178</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.2133212834596634</v>
+        <v>0.6436340808868408</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.5851173996925354</v>
+        <v>0.4847375750541687</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.6117377281188965</v>
+        <v>0.5480762720108032</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.4729233384132385</v>
+        <v>0.4705075025558472</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.2953791320323944</v>
+        <v>0.3810021877288818</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.5265879034996033</v>
+        <v>0.4849834442138672</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.4608010053634644</v>
+        <v>0.3135392367839813</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.5966947078704834</v>
+        <v>0.3405084609985352</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.3288567066192627</v>
+        <v>0.7251253128051758</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.4100537896156311</v>
+        <v>0.455298125743866</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.523874044418335</v>
+        <v>0.6206512451171875</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5297057628631592</v>
+        <v>0.5306301116943359</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.5384456515312195</v>
+        <v>0.5049592852592468</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.5027934312820435</v>
+        <v>0.4335347712039948</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.4811370372772217</v>
+        <v>0.624604344367981</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.3127312660217285</v>
+        <v>0.4437154829502106</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.1991394460201263</v>
+        <v>0.5663542747497559</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.48663729429245</v>
+        <v>0.5900990962982178</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.4381969571113586</v>
+        <v>0.662835955619812</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.6189110279083252</v>
+        <v>0.5314934253692627</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.5399258136749268</v>
+        <v>0.5541192293167114</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.6233614683151245</v>
+        <v>0.5650703907012939</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.4611505270004272</v>
+        <v>0.5482171773910522</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.5436527132987976</v>
+        <v>0.719582200050354</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.312126100063324</v>
+        <v>0.4600785970687866</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.4920777976512909</v>
+        <v>0.6140366792678833</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.6311185359954834</v>
+        <v>0.1144546717405319</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.5007669925689697</v>
+        <v>0.6045494675636292</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.4695015251636505</v>
+        <v>0.5934877395629883</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.4585674405097961</v>
+        <v>0.401841789484024</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.6702446937561035</v>
+        <v>0.5543333292007446</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.5934877395629883</v>
+        <v>0.6833282709121704</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.5517023205757141</v>
+        <v>0.2356208711862564</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.5291949510574341</v>
+        <v>0.4185349345207214</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.5281085968017578</v>
+        <v>0.4427679479122162</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5759518146514893</v>
+        <v>0.500427782535553</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.4039197266101837</v>
+        <v>0.4572167098522186</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.5709338188171387</v>
+        <v>0.4599449038505554</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.2577903866767883</v>
+        <v>0.645876407623291</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.4205964803695679</v>
+        <v>0.2905994653701782</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.3717487454414368</v>
+        <v>0.5218831300735474</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.4515761733055115</v>
+        <v>0.495439350605011</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.7174453735351562</v>
+        <v>0.5692295432090759</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.5152899622917175</v>
+        <v>0.5581192970275879</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.6357919573783875</v>
+        <v>0.3659118115901947</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.45186647772789</v>
+        <v>0.3324585258960724</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.5131638646125793</v>
+        <v>0.4658886194229126</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.6283758282661438</v>
+        <v>0.4100139141082764</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.2551113963127136</v>
+        <v>0.3075988590717316</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.5765474438667297</v>
+        <v>0.3455296754837036</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.2202349007129669</v>
+        <v>0.6212505102157593</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.5473373532295227</v>
+        <v>0.4595040082931519</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.6747076511383057</v>
+        <v>0.5782939195632935</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.4512881338596344</v>
+        <v>0.5810699462890625</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.5688920617103577</v>
+        <v>0.3243899047374725</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.3762258291244507</v>
+        <v>0.5383306741714478</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.3491390347480774</v>
+        <v>0.6674343943595886</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.3078306615352631</v>
+        <v>0.6463236212730408</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.6569996476173401</v>
+        <v>0.616655707359314</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.4790589213371277</v>
+        <v>0.5699353218078613</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.5635995864868164</v>
+        <v>0.6639398336410522</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.3583500683307648</v>
+        <v>0.4559141397476196</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.3785365223884583</v>
+        <v>0.4945109784603119</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.5250946283340454</v>
+        <v>0.3926920592784882</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.2914574146270752</v>
+        <v>0.05123074352741241</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.1280336380004883</v>
+        <v>0.1416056752204895</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.637612521648407</v>
+        <v>0.2698770463466644</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.4522941112518311</v>
+        <v>0.2746833264827728</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.6329472661018372</v>
+        <v>0.6089813709259033</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.5947767496109009</v>
+        <v>0.5189334750175476</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.5383185148239136</v>
+        <v>0.1182267442345619</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.4756194353103638</v>
+        <v>0.538690447807312</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.3292438983917236</v>
+        <v>0.5086380243301392</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.4665157496929169</v>
+        <v>0.3133353590965271</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.3780445456504822</v>
+        <v>0.4158552289009094</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.4203421473503113</v>
+        <v>0.5315454006195068</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.6458085775375366</v>
+        <v>0.4080321788787842</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.6103781461715698</v>
+        <v>0.776767909526825</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.5856053829193115</v>
+        <v>0.4511486887931824</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.5076936483383179</v>
+        <v>0.5064607262611389</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.5628009438514709</v>
+        <v>0.3974687457084656</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.6135785579681396</v>
+        <v>0.731286883354187</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.6394075751304626</v>
+        <v>0.7233157157897949</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.6552317142486572</v>
+        <v>0.7168643474578857</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.7045397758483887</v>
+        <v>0.6265950202941895</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.6681262850761414</v>
+        <v>0.7448364496231079</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.4769198298454285</v>
+        <v>0.654821515083313</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.6101669073104858</v>
+        <v>0.5234330892562866</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.5989986658096313</v>
+        <v>0.8405013084411621</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.5357596278190613</v>
+        <v>0.3976716995239258</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.7119144201278687</v>
+        <v>0.4093824625015259</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.7348048090934753</v>
+        <v>0.7035361528396606</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.7713733911514282</v>
+        <v>0.6132484078407288</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.6218023300170898</v>
+        <v>0.5658026933670044</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.6962884664535522</v>
+        <v>0.6686116456985474</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.5158118009567261</v>
+        <v>0.7089226245880127</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.5334751605987549</v>
+        <v>0.6141690015792847</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.6672381162643433</v>
+        <v>0.8110419511795044</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5505830049514771</v>
+        <v>0.5431539416313171</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.739754319190979</v>
+        <v>0.5595484972000122</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.6402907967567444</v>
+        <v>0.7410717010498047</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.5141965746879578</v>
+        <v>0.5289461612701416</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.6872057318687439</v>
+        <v>0.4727189540863037</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.5591269135475159</v>
+        <v>0.4546889662742615</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.5987022519111633</v>
+        <v>0.4411768913269043</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.499571830034256</v>
+        <v>0.3519075810909271</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.4121221601963043</v>
+        <v>0.5049721002578735</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.6544961929321289</v>
+        <v>0.6156269311904907</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.50937819480896</v>
+        <v>0.5987938046455383</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.6036520600318909</v>
+        <v>0.7137360572814941</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.6980075240135193</v>
+        <v>0.1266630589962006</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.449634313583374</v>
+        <v>0.543501079082489</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.4639484584331512</v>
+        <v>0.3712847530841827</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.3287733793258667</v>
+        <v>0.668492317199707</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.5817757844924927</v>
+        <v>0.7135797739028931</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.4984452724456787</v>
+        <v>0.548612654209137</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.4195482730865479</v>
+        <v>0.7138724327087402</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.3279612064361572</v>
+        <v>0.592034637928009</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.3539080619812012</v>
+        <v>0.5429444909095764</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.6208164691925049</v>
+        <v>0.401046484708786</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.4987038969993591</v>
+        <v>0.5150627493858337</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.4458021521568298</v>
+        <v>0.5313801169395447</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.2674353718757629</v>
+        <v>0.5021304488182068</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.4594922363758087</v>
+        <v>0.6616018414497375</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.4087314009666443</v>
+        <v>0.3509668409824371</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.5408759713172913</v>
+        <v>0.3117470741271973</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.1502426862716675</v>
+        <v>0.4732962250709534</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.397789478302002</v>
+        <v>0.503650426864624</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.5357591509819031</v>
+        <v>0.5033645629882812</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.6203102469444275</v>
+        <v>0.4197413325309753</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.3828181624412537</v>
+        <v>0.2517394721508026</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.5128957629203796</v>
+        <v>0.2715261876583099</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.6099224090576172</v>
+        <v>0.3989769518375397</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.5450041890144348</v>
+        <v>0.3676620125770569</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.3709759414196014</v>
+        <v>0.2895398736000061</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.2279988527297974</v>
+        <v>0.4891645014286041</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.4221978783607483</v>
+        <v>0.4224794507026672</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.6082369685173035</v>
+        <v>0.4098601043224335</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.4958017766475677</v>
+        <v>0.4039253294467926</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.4880731999874115</v>
+        <v>0.5310485363006592</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.6468315720558167</v>
+        <v>0.3062445819377899</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made Edits to gemma_3
</commit_message>
<xml_diff>
--- a/results/Semantic_Similarities_Gemma_untrained.xlsx
+++ b/results/Semantic_Similarities_Gemma_untrained.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6920520663261414</v>
+        <v>0.5631184577941895</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.729717493057251</v>
+        <v>0.6051477193832397</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.6769880056381226</v>
+        <v>0.5314805507659912</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.3804360330104828</v>
+        <v>0.5091396570205688</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4451932609081268</v>
+        <v>0.4426529109477997</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.5703897476196289</v>
+        <v>0.2850387096405029</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.5163048505783081</v>
+        <v>0.3270883560180664</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.5279713273048401</v>
+        <v>0.7124536037445068</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6451247334480286</v>
+        <v>0.3815630078315735</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.5678476691246033</v>
+        <v>0.7018503546714783</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.7257301807403564</v>
+        <v>0.6045142412185669</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.4742555022239685</v>
+        <v>0.4144102334976196</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.5271262526512146</v>
+        <v>0.6402942538261414</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.4080379903316498</v>
+        <v>0.5307226181030273</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4415383338928223</v>
+        <v>0.5813566446304321</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5665831565856934</v>
+        <v>0.5454379320144653</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3711598515510559</v>
+        <v>0.5775209665298462</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2795150279998779</v>
+        <v>0.2288756817579269</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.5485844612121582</v>
+        <v>0.6627068519592285</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5284099578857422</v>
+        <v>0.613127589225769</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3018908202648163</v>
+        <v>0.3183037936687469</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.4606550931930542</v>
+        <v>0.5770862102508545</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.6264884471893311</v>
+        <v>0.5159566402435303</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.6407639384269714</v>
+        <v>0.3553860187530518</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.6765548586845398</v>
+        <v>0.5739498138427734</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.5343475341796875</v>
+        <v>0.5516995191574097</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.5300296545028687</v>
+        <v>0.4914547801017761</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.3813424110412598</v>
+        <v>0.5148975849151611</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.7179755568504333</v>
+        <v>0.6550814509391785</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.4929227530956268</v>
+        <v>0.4856145083904266</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.4931705892086029</v>
+        <v>0.5328034162521362</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.465474009513855</v>
+        <v>0.5025287866592407</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.6304359436035156</v>
+        <v>0.2844935953617096</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5595799684524536</v>
+        <v>0.5536140203475952</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5026155710220337</v>
+        <v>0.4936468601226807</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.3131013512611389</v>
+        <v>0.6326751112937927</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.62077397108078</v>
+        <v>0.4963562786579132</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.689457893371582</v>
+        <v>0.6056767702102661</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.5764554738998413</v>
+        <v>0.689488410949707</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6119536161422729</v>
+        <v>0.6220400333404541</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.3172469437122345</v>
+        <v>0.4731249809265137</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.3223828971385956</v>
+        <v>0.5913683176040649</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.3950381875038147</v>
+        <v>0.5536448955535889</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.4986931681632996</v>
+        <v>0.4412475228309631</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.5837039947509766</v>
+        <v>0.4159185290336609</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.6700018644332886</v>
+        <v>0.4118554592132568</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.4231172204017639</v>
+        <v>0.6189916729927063</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.4077571332454681</v>
+        <v>0.439109742641449</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.3140339255332947</v>
+        <v>0.4711459577083588</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.608534574508667</v>
+        <v>0.5102269649505615</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.3757619857788086</v>
+        <v>0.3439280688762665</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.3638131022453308</v>
+        <v>0.4632894098758698</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.464464008808136</v>
+        <v>0.2925341427326202</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.4007188677787781</v>
+        <v>0.3488527834415436</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.5289671421051025</v>
+        <v>0.2490301132202148</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.4455665647983551</v>
+        <v>0.5495445132255554</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.4342573285102844</v>
+        <v>0.203346312046051</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.5671559572219849</v>
+        <v>0.7429825067520142</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.5466420650482178</v>
+        <v>0.6061481237411499</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.6436340808868408</v>
+        <v>0.2675977945327759</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.4847375750541687</v>
+        <v>0.4256055951118469</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.5480762720108032</v>
+        <v>0.4481513202190399</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.4705075025558472</v>
+        <v>0.5986588001251221</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.3810021877288818</v>
+        <v>0.4264119565486908</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.4849834442138672</v>
+        <v>0.4794977605342865</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.3135392367839813</v>
+        <v>0.5641944408416748</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.3405084609985352</v>
+        <v>0.5332262516021729</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.7251253128051758</v>
+        <v>0.5762537717819214</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.455298125743866</v>
+        <v>0.4060788750648499</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.6206512451171875</v>
+        <v>0.4635285139083862</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5306301116943359</v>
+        <v>0.5286709666252136</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.5049592852592468</v>
+        <v>0.4943705201148987</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.4335347712039948</v>
+        <v>0.4351374208927155</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.624604344367981</v>
+        <v>0.3981055021286011</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.4437154829502106</v>
+        <v>0.3940036296844482</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.5663542747497559</v>
+        <v>0.5257856845855713</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.5900990962982178</v>
+        <v>0.4537406265735626</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.662835955619812</v>
+        <v>0.397861510515213</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.5314934253692627</v>
+        <v>0.3933637142181396</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.5541192293167114</v>
+        <v>0.4568235874176025</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.5650703907012939</v>
+        <v>0.375805526971817</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.5482171773910522</v>
+        <v>0.6529560089111328</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.719582200050354</v>
+        <v>0.702094554901123</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.4600785970687866</v>
+        <v>0.6331790685653687</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.6140366792678833</v>
+        <v>0.54201740026474</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.1144546717405319</v>
+        <v>0.352821558713913</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.6045494675636292</v>
+        <v>0.2992914617061615</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5934877395629883</v>
+        <v>0.5189078450202942</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.401841789484024</v>
+        <v>0.3015949726104736</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.5543333292007446</v>
+        <v>0.6009635925292969</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.6833282709121704</v>
+        <v>0.4780917167663574</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.2356208711862564</v>
+        <v>0.5678498148918152</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.4185349345207214</v>
+        <v>0.2788923978805542</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.4427679479122162</v>
+        <v>0.3707678914070129</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.500427782535553</v>
+        <v>0.3649381995201111</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.4572167098522186</v>
+        <v>0.4507867693901062</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.4599449038505554</v>
+        <v>0.355681836605072</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.645876407623291</v>
+        <v>0.6160184144973755</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.2905994653701782</v>
+        <v>0.2593239545822144</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.5218831300735474</v>
+        <v>0.6450899839401245</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.495439350605011</v>
+        <v>0.6165976524353027</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.5692295432090759</v>
+        <v>0.6021537184715271</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.5581192970275879</v>
+        <v>0.5175410509109497</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.3659118115901947</v>
+        <v>0.3225276172161102</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.3324585258960724</v>
+        <v>0.4526441991329193</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.4658886194229126</v>
+        <v>0.4525653719902039</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.4100139141082764</v>
+        <v>0.4024764895439148</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.3075988590717316</v>
+        <v>0.5647408962249756</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.3455296754837036</v>
+        <v>0.6272668242454529</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.6212505102157593</v>
+        <v>0.3267099261283875</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.4595040082931519</v>
+        <v>0.4945138394832611</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.5782939195632935</v>
+        <v>0.2702999114990234</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.5810699462890625</v>
+        <v>0.3394745588302612</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.3243899047374725</v>
+        <v>0.4972372651100159</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.5383306741714478</v>
+        <v>0.351438045501709</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.6674343943595886</v>
+        <v>0.3494727611541748</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.6463236212730408</v>
+        <v>0.5455836057662964</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.616655707359314</v>
+        <v>0.5428449511528015</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.5699353218078613</v>
+        <v>0.4049950242042542</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.6639398336410522</v>
+        <v>0.3806173205375671</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.4559141397476196</v>
+        <v>0.5821816921234131</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.4945109784603119</v>
+        <v>0.4505662620067596</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.3926920592784882</v>
+        <v>0.3978868126869202</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.05123074352741241</v>
+        <v>0.5617725849151611</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.1416056752204895</v>
+        <v>0.5110410451889038</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.2698770463466644</v>
+        <v>0.6139803528785706</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.2746833264827728</v>
+        <v>0.5411211848258972</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.6089813709259033</v>
+        <v>0.393460214138031</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.5189334750175476</v>
+        <v>0.5490926504135132</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.1182267442345619</v>
+        <v>0.4051096141338348</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.538690447807312</v>
+        <v>0.3824748992919922</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.5086380243301392</v>
+        <v>0.6322949528694153</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.3133353590965271</v>
+        <v>0.4613402187824249</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.4158552289009094</v>
+        <v>0.0438980758190155</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.5315454006195068</v>
+        <v>0.1974304765462875</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.4080321788787842</v>
+        <v>0.2942083477973938</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.776767909526825</v>
+        <v>0.1598467379808426</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.4511486887931824</v>
+        <v>0.2128930389881134</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.5064607262611389</v>
+        <v>0.7444181442260742</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.3974687457084656</v>
+        <v>0.5255957841873169</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.731286883354187</v>
+        <v>0.7095434069633484</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.7233157157897949</v>
+        <v>0.6591542959213257</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.7168643474578857</v>
+        <v>0.8043602108955383</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.6265950202941895</v>
+        <v>0.671684205532074</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.7448364496231079</v>
+        <v>0.3488388657569885</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.654821515083313</v>
+        <v>0.6563517451286316</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.5234330892562866</v>
+        <v>0.4511405229568481</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.8405013084411621</v>
+        <v>0.7089884877204895</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.3976716995239258</v>
+        <v>0.5001003742218018</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.4093824625015259</v>
+        <v>0.4677178561687469</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.7035361528396606</v>
+        <v>0.816752016544342</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.6132484078407288</v>
+        <v>0.4496606588363647</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.5658026933670044</v>
+        <v>0.7533355951309204</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.6686116456985474</v>
+        <v>0.5491630434989929</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.7089226245880127</v>
+        <v>0.7238004207611084</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.6141690015792847</v>
+        <v>0.6778205633163452</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.8110419511795044</v>
+        <v>0.5607990026473999</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5431539416313171</v>
+        <v>0.5592436790466309</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.5595484972000122</v>
+        <v>0.6842960715293884</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.7410717010498047</v>
+        <v>0.5403964519500732</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.5289461612701416</v>
+        <v>0.6091476678848267</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.4727189540863037</v>
+        <v>0.4595294594764709</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.4546889662742615</v>
+        <v>0.4891339242458344</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.4411768913269043</v>
+        <v>0.6032525300979614</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.3519075810909271</v>
+        <v>0.4223189055919647</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.5049721002578735</v>
+        <v>0.4924927949905396</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.6156269311904907</v>
+        <v>0.7211182713508606</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.5987938046455383</v>
+        <v>0.7141708135604858</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.7137360572814941</v>
+        <v>0.6014024019241333</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.1266630589962006</v>
+        <v>0.60719233751297</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.543501079082489</v>
+        <v>0.5730077028274536</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.3712847530841827</v>
+        <v>0.6519920825958252</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.668492317199707</v>
+        <v>0.66038978099823</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.7135797739028931</v>
+        <v>0.6279056072235107</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.548612654209137</v>
+        <v>0.511924147605896</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.7138724327087402</v>
+        <v>0.6953569054603577</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.592034637928009</v>
+        <v>0.4538717567920685</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.5429444909095764</v>
+        <v>0.5032078623771667</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.401046484708786</v>
+        <v>0.1857385635375977</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.5150627493858337</v>
+        <v>0.4040490388870239</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.5313801169395447</v>
+        <v>0.3870758712291718</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.5021304488182068</v>
+        <v>0.2714062929153442</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.6616018414497375</v>
+        <v>0.4721464216709137</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.3509668409824371</v>
+        <v>0.3863331079483032</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.3117470741271973</v>
+        <v>0.5272349715232849</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.4732962250709534</v>
+        <v>0.5074800848960876</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.503650426864624</v>
+        <v>0.2865062057971954</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.5033645629882812</v>
+        <v>0.342124342918396</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.4197413325309753</v>
+        <v>0.5260173082351685</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.2517394721508026</v>
+        <v>0.3815919458866119</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.2715261876583099</v>
+        <v>0.5066900849342346</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.3989769518375397</v>
+        <v>0.5113481283187866</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.3676620125770569</v>
+        <v>0.4574733972549438</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.2895398736000061</v>
+        <v>0.5082167387008667</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.4891645014286041</v>
+        <v>0.3412750363349915</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.4224794507026672</v>
+        <v>0.5091410279273987</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.4098601043224335</v>
+        <v>0.5446195602416992</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.4039253294467926</v>
+        <v>0.5068828463554382</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.5310485363006592</v>
+        <v>0.3581134080886841</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.3062445819377899</v>
+        <v>0.3551633358001709</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on textual entailment problem
</commit_message>
<xml_diff>
--- a/results/Semantic_Similarities_Gemma_untrained.xlsx
+++ b/results/Semantic_Similarities_Gemma_untrained.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.5631184577941895</v>
+        <v>0.7319974899291992</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.6051477193832397</v>
+        <v>0.4967910945415497</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5314805507659912</v>
+        <v>0.8961496353149414</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.5091396570205688</v>
+        <v>0.2741787433624268</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4426529109477997</v>
+        <v>0.8295943737030029</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.2850387096405029</v>
+        <v>0.6488519906997681</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3270883560180664</v>
+        <v>0.8663877844810486</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.7124536037445068</v>
+        <v>0.6541480422019958</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.3815630078315735</v>
+        <v>0.6322076320648193</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.7018503546714783</v>
+        <v>0.8830806612968445</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6045142412185669</v>
+        <v>0.1194158643484116</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.4144102334976196</v>
+        <v>0.08379790931940079</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.6402942538261414</v>
+        <v>0.4607940912246704</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5307226181030273</v>
+        <v>0.8825771808624268</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5813566446304321</v>
+        <v>0.5266714692115784</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.5454379320144653</v>
+        <v>0.670512855052948</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.5775209665298462</v>
+        <v>0.3176763653755188</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.2288756817579269</v>
+        <v>0.7920719385147095</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.6627068519592285</v>
+        <v>-0.02148962393403053</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.613127589225769</v>
+        <v>0.5962247252464294</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.3183037936687469</v>
+        <v>0.6744462251663208</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.5770862102508545</v>
+        <v>0.7662100791931152</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5159566402435303</v>
+        <v>0.5044233798980713</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>0.3553860187530518</v>
+        <v>-0.0351753868162632</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.5739498138427734</v>
+        <v>0.533031702041626</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.5516995191574097</v>
+        <v>0.8062756061553955</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.4914547801017761</v>
+        <v>0.8955717086791992</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.5148975849151611</v>
+        <v>0.8860354423522949</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.6550814509391785</v>
+        <v>0.6790879964828491</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.4856145083904266</v>
+        <v>0.827057421207428</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.5328034162521362</v>
+        <v>0.8466249704360962</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.5025287866592407</v>
+        <v>0.5201642513275146</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.2844935953617096</v>
+        <v>0.6963426470756531</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.5536140203475952</v>
+        <v>0.7806293964385986</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.4936468601226807</v>
+        <v>0.5131650567054749</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.6326751112937927</v>
+        <v>0.6721723079681396</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.4963562786579132</v>
+        <v>0.9480384588241577</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.6056767702102661</v>
+        <v>0.9204800724983215</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.689488410949707</v>
+        <v>0.3357254862785339</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.6220400333404541</v>
+        <v>0.5343362092971802</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.4731249809265137</v>
+        <v>0.8284595012664795</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.5913683176040649</v>
+        <v>0.6556806564331055</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.5536448955535889</v>
+        <v>0.5722887516021729</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.4412475228309631</v>
+        <v>0.5298775434494019</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.4159185290336609</v>
+        <v>0.7591912150382996</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>0.4118554592132568</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.6189916729927063</v>
+        <v>0.6444385051727295</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.439109742641449</v>
+        <v>0.548100471496582</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.4711459577083588</v>
+        <v>0.7492806911468506</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.5102269649505615</v>
+        <v>0.6149642467498779</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.3439280688762665</v>
+        <v>0.7647819519042969</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.4632894098758698</v>
+        <v>0.6754446029663086</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.2925341427326202</v>
+        <v>0.6569817066192627</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.3488527834415436</v>
+        <v>0.2992706298828125</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.2490301132202148</v>
+        <v>0.2558636665344238</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.5495445132255554</v>
+        <v>0.6690149903297424</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.203346312046051</v>
+        <v>0.5735132694244385</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.7429825067520142</v>
+        <v>0.6833854913711548</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.6061481237411499</v>
+        <v>0.4717593193054199</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.2675977945327759</v>
+        <v>0.9118872284889221</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.4256055951118469</v>
+        <v>0.6943370699882507</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.4481513202190399</v>
+        <v>0.6456588506698608</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.5986588001251221</v>
+        <v>0.6204570531845093</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.4264119565486908</v>
+        <v>0.7096143364906311</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.4794977605342865</v>
+        <v>0.5855088829994202</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.5641944408416748</v>
+        <v>0.615328311920166</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.5332262516021729</v>
+        <v>0.8558082580566406</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.5762537717819214</v>
+        <v>0.897997260093689</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.4060788750648499</v>
+        <v>0.8015692830085754</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.4635285139083862</v>
+        <v>0.7647612690925598</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5286709666252136</v>
+        <v>0.5500362515449524</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.4943705201148987</v>
+        <v>0.6820584535598755</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.4351374208927155</v>
+        <v>0.8657664060592651</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.3981055021286011</v>
+        <v>0.7496740818023682</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.3940036296844482</v>
+        <v>0.7879183292388916</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.5257856845855713</v>
+        <v>0.7377111911773682</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.4537406265735626</v>
+        <v>0.5276908278465271</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.397861510515213</v>
+        <v>0.5194127559661865</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.3933637142181396</v>
+        <v>0.6158688068389893</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.4568235874176025</v>
+        <v>0.01206494122743607</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.375805526971817</v>
+        <v>0.1141128838062286</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.6529560089111328</v>
+        <v>0.5688951015472412</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.702094554901123</v>
+        <v>0.6487776041030884</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.6331790685653687</v>
+        <v>0.5651538372039795</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.54201740026474</v>
+        <v>0.4465360343456268</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.352821558713913</v>
+        <v>0.8643482327461243</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.2992914617061615</v>
+        <v>0.330811619758606</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5189078450202942</v>
+        <v>0.5682190656661987</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.3015949726104736</v>
+        <v>0.4893761277198792</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.6009635925292969</v>
+        <v>0.6150315403938293</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.4780917167663574</v>
+        <v>0.6345044374465942</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.5678498148918152</v>
+        <v>0.6692838668823242</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.2788923978805542</v>
+        <v>0.689927875995636</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.3707678914070129</v>
+        <v>0.5324441194534302</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.3649381995201111</v>
+        <v>0.5885096192359924</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.4507867693901062</v>
+        <v>0.6161863803863525</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.355681836605072</v>
+        <v>0.4874723553657532</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.6160184144973755</v>
+        <v>0.8123556971549988</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.2593239545822144</v>
+        <v>0.7857388257980347</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.6450899839401245</v>
+        <v>0.7924134135246277</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.6165976524353027</v>
+        <v>0.6665103435516357</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.6021537184715271</v>
+        <v>0.5966357588768005</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.5175410509109497</v>
+        <v>0.4950587153434753</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.3225276172161102</v>
+        <v>0.6949255466461182</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.4526441991329193</v>
+        <v>0.282066136598587</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.4525653719902039</v>
+        <v>0.7550283074378967</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.4024764895439148</v>
+        <v>0.6412414312362671</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.5647408962249756</v>
+        <v>0.3455393314361572</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.6272668242454529</v>
+        <v>0.6001375913619995</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.3267099261283875</v>
+        <v>0.7157982587814331</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.4945138394832611</v>
+        <v>0.07818658649921417</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.2702999114990234</v>
+        <v>0.5099846720695496</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.3394745588302612</v>
+        <v>0.8173660039901733</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.4972372651100159</v>
+        <v>0.4348182678222656</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.351438045501709</v>
+        <v>0.5293052196502686</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.3494727611541748</v>
+        <v>0.5736711025238037</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.5455836057662964</v>
+        <v>0.5202480554580688</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.5428449511528015</v>
+        <v>0.691972017288208</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.4049950242042542</v>
+        <v>0.5738469362258911</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.3806173205375671</v>
+        <v>0.6944172382354736</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.5821816921234131</v>
+        <v>0.8049269914627075</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.4505662620067596</v>
+        <v>0.8756381869316101</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.3978868126869202</v>
+        <v>0.581815779209137</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.5617725849151611</v>
+        <v>0.1633659303188324</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.5110410451889038</v>
+        <v>0.2244278937578201</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.6139803528785706</v>
+        <v>0.2039750069379807</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.5411211848258972</v>
+        <v>0.8758256435394287</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.393460214138031</v>
+        <v>0.6657535433769226</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.5490926504135132</v>
+        <v>0.2764238119125366</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.4051096141338348</v>
+        <v>0.4329104721546173</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.3824748992919922</v>
+        <v>0.3568612933158875</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.6322949528694153</v>
+        <v>0.6780085563659668</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.4613402187824249</v>
+        <v>0.6670798063278198</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.0438980758190155</v>
+        <v>0.7897450923919678</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.1974304765462875</v>
+        <v>0.6550347805023193</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.2942083477973938</v>
+        <v>0.916786253452301</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.1598467379808426</v>
+        <v>0.5931817889213562</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.2128930389881134</v>
+        <v>0.003507103770971298</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.7444181442260742</v>
+        <v>0.4980825185775757</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.5255957841873169</v>
+        <v>0.3262921571731567</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.7095434069633484</v>
+        <v>0.6091154813766479</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.6591542959213257</v>
+        <v>0.4599698185920715</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.8043602108955383</v>
+        <v>0.6016952395439148</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.671684205532074</v>
+        <v>0.5259081721305847</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.3488388657569885</v>
+        <v>0.7240345478057861</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.6563517451286316</v>
+        <v>0.6903635263442993</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.4511405229568481</v>
+        <v>0.6666012406349182</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.7089884877204895</v>
+        <v>0.6445336937904358</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.5001003742218018</v>
+        <v>0.6941819190979004</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.4677178561687469</v>
+        <v>0.7563785314559937</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.816752016544342</v>
+        <v>0.7091559171676636</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.4496606588363647</v>
+        <v>0.8520588874816895</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>0.7533355951309204</v>
+        <v>-0.01526674628257751</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.5491630434989929</v>
+        <v>0.6388297080993652</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.7238004207611084</v>
+        <v>0.7464070320129395</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.6778205633163452</v>
+        <v>0.7501164078712463</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.5607990026473999</v>
+        <v>0.557317316532135</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.5592436790466309</v>
+        <v>0.06462706625461578</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.6842960715293884</v>
+        <v>0.4653899073600769</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.5403964519500732</v>
+        <v>0.0691843181848526</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.6091476678848267</v>
+        <v>0.16939377784729</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.4595294594764709</v>
+        <v>0.6979347467422485</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.4891339242458344</v>
+        <v>0.7155879139900208</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.6032525300979614</v>
+        <v>0.7694939374923706</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.4223189055919647</v>
+        <v>0.6863052845001221</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.4924927949905396</v>
+        <v>0.3957986235618591</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.7211182713508606</v>
+        <v>0.259017139673233</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.7141708135604858</v>
+        <v>0.7460633516311646</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.6014024019241333</v>
+        <v>0.5808224678039551</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.60719233751297</v>
+        <v>0.3524478375911713</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.5730077028274536</v>
+        <v>0.6563334465026855</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.6519920825958252</v>
+        <v>0.3625905811786652</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.66038978099823</v>
+        <v>0.556209921836853</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.6279056072235107</v>
+        <v>0.779334545135498</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.511924147605896</v>
+        <v>0.6573541760444641</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.6953569054603577</v>
+        <v>0.4356926083564758</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.4538717567920685</v>
+        <v>0.6598786115646362</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.5032078623771667</v>
+        <v>0.08071070164442062</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.1857385635375977</v>
+        <v>0.5030912160873413</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.4040490388870239</v>
+        <v>0.3984063863754272</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.3870758712291718</v>
+        <v>0.695335865020752</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.2714062929153442</v>
+        <v>0.6452840566635132</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.4721464216709137</v>
+        <v>0.3681568801403046</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.3863331079483032</v>
+        <v>0.6338929533958435</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.5272349715232849</v>
+        <v>0.3899437785148621</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.5074800848960876</v>
+        <v>0.4644167721271515</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.2865062057971954</v>
+        <v>0.4627735316753387</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.342124342918396</v>
+        <v>0.5749266147613525</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.5260173082351685</v>
+        <v>0.6312191486358643</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.3815919458866119</v>
+        <v>0.5915489196777344</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.5066900849342346</v>
+        <v>0.8803046345710754</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.5113481283187866</v>
+        <v>0.3883032202720642</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.4574733972549438</v>
+        <v>0.6913920640945435</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.5082167387008667</v>
+        <v>0.6121551990509033</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.3412750363349915</v>
+        <v>0.6827068328857422</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.5091410279273987</v>
+        <v>0.7839042544364929</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.5446195602416992</v>
+        <v>0.6297519207000732</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.5068828463554382</v>
+        <v>0.5138713121414185</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.3581134080886841</v>
+        <v>0.3976235389709473</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.3551633358001709</v>
+        <v>0.6419792175292969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempted to train Gemma Finetune
</commit_message>
<xml_diff>
--- a/results/Semantic_Similarities_Gemma_untrained.xlsx
+++ b/results/Semantic_Similarities_Gemma_untrained.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.7319974899291992</v>
+        <v>0.1337130069732666</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.4967910945415497</v>
+        <v>0.01194232422858477</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.8961496353149414</v>
+        <v>0.03822752088308334</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2741787433624268</v>
+        <v>-0.03966856747865677</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.8295943737030029</v>
+        <v>0.08881343901157379</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6488519906997681</v>
+        <v>0.02483552694320679</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.8663877844810486</v>
+        <v>0.1052547171711922</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.6541480422019958</v>
+        <v>0.120028480887413</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.6322076320648193</v>
+        <v>0.1080748736858368</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8830806612968445</v>
+        <v>0.06621682643890381</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1194158643484116</v>
+        <v>0.09913419932126999</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.08379790931940079</v>
+        <v>0.07487849146127701</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.4607940912246704</v>
+        <v>0.05794435739517212</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.8825771808624268</v>
+        <v>0.1135500222444534</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.5266714692115784</v>
+        <v>0.1437799334526062</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.670512855052948</v>
+        <v>0.006930546835064888</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.3176763653755188</v>
+        <v>0.02288063429296017</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.7920719385147095</v>
+        <v>0.04012411460280418</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>-0.02148962393403053</v>
+        <v>0.1582256853580475</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.5962247252464294</v>
+        <v>0.1686297357082367</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>0.6744462251663208</v>
+        <v>0.07941283285617828</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>0.7662100791931152</v>
+        <v>-0.08948665857315063</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>0.5044233798980713</v>
+        <v>0.1202997118234634</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>-0.0351753868162632</v>
+        <v>-0.0002254033461213112</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>0.533031702041626</v>
+        <v>-0.1204040050506592</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8062756061553955</v>
+        <v>0.2407238632440567</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>0.8955717086791992</v>
+        <v>-0.03013794124126434</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>0.8860354423522949</v>
+        <v>-0.04664886370301247</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>0.6790879964828491</v>
+        <v>0.09317386895418167</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>0.827057421207428</v>
+        <v>0.1237642094492912</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>0.8466249704360962</v>
+        <v>-0.006163325160741806</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>0.5201642513275146</v>
+        <v>0.1908396780490875</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>0.6963426470756531</v>
+        <v>0.1169669404625893</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>0.7806293964385986</v>
+        <v>0.1323374807834625</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>0.5131650567054749</v>
+        <v>0.1088209897279739</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>0.6721723079681396</v>
+        <v>0.03900296241044998</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>0.9480384588241577</v>
+        <v>0.0246388278901577</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>0.9204800724983215</v>
+        <v>-0.02129474096000195</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>0.3357254862785339</v>
+        <v>0.07719183713197708</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>0.5343362092971802</v>
+        <v>-0.08350475132465363</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>0.8284595012664795</v>
+        <v>-0.0005329642444849014</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>0.6556806564331055</v>
+        <v>0.01508797146379948</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>0.5722887516021729</v>
+        <v>-0.07014082372188568</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>0.5298775434494019</v>
+        <v>-0.02738713473081589</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>0.7591912150382996</v>
+        <v>0.01876363903284073</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>1</v>
+        <v>0.002671496942639351</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>0.6444385051727295</v>
+        <v>0.07751298695802689</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>0.548100471496582</v>
+        <v>0.07404179871082306</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>0.7492806911468506</v>
+        <v>0.4023616015911102</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>0.6149642467498779</v>
+        <v>0.06005425751209259</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>0.7647819519042969</v>
+        <v>0.08357451111078262</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>0.6754446029663086</v>
+        <v>0.002672199159860611</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>0.6569817066192627</v>
+        <v>0.07076596468687057</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>0.2992706298828125</v>
+        <v>0.0775318443775177</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>0.2558636665344238</v>
+        <v>0.01782641746103764</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>0.6690149903297424</v>
+        <v>0.1576853692531586</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>0.5735132694244385</v>
+        <v>0.1006143242120743</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>0.6833854913711548</v>
+        <v>0.04870180040597916</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>0.4717593193054199</v>
+        <v>0.03332386910915375</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>0.9118872284889221</v>
+        <v>0.1028463840484619</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>0.6943370699882507</v>
+        <v>0.02230880595743656</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>0.6456588506698608</v>
+        <v>0.002937975339591503</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>0.6204570531845093</v>
+        <v>0.2426291406154633</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>0.7096143364906311</v>
+        <v>0.01074299030005932</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>0.5855088829994202</v>
+        <v>0.005498990416526794</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>0.615328311920166</v>
+        <v>0.1862244009971619</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>0.8558082580566406</v>
+        <v>0.03947911038994789</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>0.897997260093689</v>
+        <v>0.1035525649785995</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>0.8015692830085754</v>
+        <v>-0.08226727694272995</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>0.7647612690925598</v>
+        <v>-0.07494188845157623</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>0.5500362515449524</v>
+        <v>0.02654918096959591</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>0.6820584535598755</v>
+        <v>-0.04222141206264496</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>0.8657664060592651</v>
+        <v>-0.02174246311187744</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>0.7496740818023682</v>
+        <v>0.1011256948113441</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>0.7879183292388916</v>
+        <v>0.07547385990619659</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>0.7377111911773682</v>
+        <v>0.08669683337211609</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>0.5276908278465271</v>
+        <v>0.068817138671875</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>0.5194127559661865</v>
+        <v>0.06734786182641983</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>0.6158688068389893</v>
+        <v>-0.1285205036401749</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>0.01206494122743607</v>
+        <v>0.09335104376077652</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>0.1141128838062286</v>
+        <v>-0.06261681020259857</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>0.5688951015472412</v>
+        <v>0.1374115794897079</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>0.6487776041030884</v>
+        <v>0.008609483018517494</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>0.5651538372039795</v>
+        <v>-0.004463400691747665</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>0.4465360343456268</v>
+        <v>0.04557641968131065</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>0.8643482327461243</v>
+        <v>0.1741210669279099</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>0.330811619758606</v>
+        <v>0.1181063801050186</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>0.5682190656661987</v>
+        <v>-0.04910839349031448</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>0.4893761277198792</v>
+        <v>0.06414060294628143</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>0.6150315403938293</v>
+        <v>0.003813996911048889</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>0.6345044374465942</v>
+        <v>-0.0185021385550499</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>0.6692838668823242</v>
+        <v>0.1657291650772095</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>0.689927875995636</v>
+        <v>-0.122063159942627</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>0.5324441194534302</v>
+        <v>0.04688186198472977</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>0.5885096192359924</v>
+        <v>0.09028782695531845</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>0.6161863803863525</v>
+        <v>0.04006288945674896</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>0.4874723553657532</v>
+        <v>-0.09477437287569046</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>0.8123556971549988</v>
+        <v>-0.07437723875045776</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>0.7857388257980347</v>
+        <v>-0.007271640002727509</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>0.7924134135246277</v>
+        <v>0.2272249907255173</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>0.6665103435516357</v>
+        <v>0.06399457156658173</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>0.5966357588768005</v>
+        <v>-0.05332828685641289</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>0.4950587153434753</v>
+        <v>0.004489865154027939</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>0.6949255466461182</v>
+        <v>0.1122548431158066</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>0.282066136598587</v>
+        <v>0.04482964798808098</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>0.7550283074378967</v>
+        <v>0.001899274066090584</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>0.6412414312362671</v>
+        <v>0.1326861381530762</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>0.3455393314361572</v>
+        <v>-0.01680421829223633</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>0.6001375913619995</v>
+        <v>-0.01778151839971542</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>0.7157982587814331</v>
+        <v>-0.01288018096238375</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>0.07818658649921417</v>
+        <v>0.09518531709909439</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>0.5099846720695496</v>
+        <v>0.007503651082515717</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>0.8173660039901733</v>
+        <v>-0.08933139592409134</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>0.4348182678222656</v>
+        <v>0.09709639847278595</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>0.5293052196502686</v>
+        <v>0.04233472794294357</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>0.5736711025238037</v>
+        <v>0.01533191278576851</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>0.5202480554580688</v>
+        <v>0.1279513239860535</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>0.691972017288208</v>
+        <v>-0.001565046608448029</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>0.5738469362258911</v>
+        <v>0.1659857332706451</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>0.6944172382354736</v>
+        <v>-0.05381184071302414</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>0.8049269914627075</v>
+        <v>0.04116277396678925</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>0.8756381869316101</v>
+        <v>-0.08696199953556061</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>0.581815779209137</v>
+        <v>-0.01623211987316608</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>0.1633659303188324</v>
+        <v>-0.0417897142469883</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>0.2244278937578201</v>
+        <v>-0.1444575935602188</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>0.2039750069379807</v>
+        <v>-0.007735438644886017</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>0.8758256435394287</v>
+        <v>-0.06488575041294098</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>0.6657535433769226</v>
+        <v>-0.1072858795523643</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>0.2764238119125366</v>
+        <v>-0.01699330285191536</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>0.4329104721546173</v>
+        <v>0.2417561113834381</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>0.3568612933158875</v>
+        <v>-0.01224410906434059</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>0.6780085563659668</v>
+        <v>0.06512216478586197</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>0.6670798063278198</v>
+        <v>0.03354191780090332</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>0.7897450923919678</v>
+        <v>0.06473542004823685</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>0.6550347805023193</v>
+        <v>-0.01384520344436169</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>0.916786253452301</v>
+        <v>0.1744602918624878</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>0.5931817889213562</v>
+        <v>0.002271987497806549</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>0.003507103770971298</v>
+        <v>0.02528553828597069</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>0.4980825185775757</v>
+        <v>0.02759867906570435</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>0.3262921571731567</v>
+        <v>0.1411304771900177</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>0.6091154813766479</v>
+        <v>0.04633217304944992</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>0.4599698185920715</v>
+        <v>0.02429861202836037</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>0.6016952395439148</v>
+        <v>-0.04841826111078262</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>0.5259081721305847</v>
+        <v>-0.1032991707324982</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>0.7240345478057861</v>
+        <v>0.009977996349334717</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>0.6903635263442993</v>
+        <v>0.06400995701551437</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>0.6666012406349182</v>
+        <v>-0.05651479214429855</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>0.6445336937904358</v>
+        <v>0.07555735111236572</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>0.6941819190979004</v>
+        <v>0.3553340435028076</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>0.7563785314559937</v>
+        <v>-0.008839418180286884</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>0.7091559171676636</v>
+        <v>-0.01380608975887299</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>0.8520588874816895</v>
+        <v>-0.08394023776054382</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>-0.01526674628257751</v>
+        <v>0.05371510982513428</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>0.6388297080993652</v>
+        <v>0.05560779571533203</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>0.7464070320129395</v>
+        <v>0.2357340008020401</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>0.7501164078712463</v>
+        <v>-0.08583450317382812</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>0.557317316532135</v>
+        <v>-0.02675044909119606</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>0.06462706625461578</v>
+        <v>0.1456594467163086</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>0.4653899073600769</v>
+        <v>0.08890543133020401</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>0.0691843181848526</v>
+        <v>-0.05915053188800812</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>0.16939377784729</v>
+        <v>0.05268723890185356</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>0.6979347467422485</v>
+        <v>-0.02536959201097488</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>0.7155879139900208</v>
+        <v>0.03750300034880638</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>0.7694939374923706</v>
+        <v>0.1596988141536713</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>0.6863052845001221</v>
+        <v>0.0872800350189209</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>0.3957986235618591</v>
+        <v>0.002068495377898216</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>0.259017139673233</v>
+        <v>0.05468908697366714</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>0.7460633516311646</v>
+        <v>0.08030027151107788</v>
       </c>
     </row>
     <row r="170">
@@ -1787,7 +1787,7 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>0.5808224678039551</v>
+        <v>0.1464872658252716</v>
       </c>
     </row>
     <row r="171">
@@ -1795,7 +1795,7 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>0.3524478375911713</v>
+        <v>0.009046174585819244</v>
       </c>
     </row>
     <row r="172">
@@ -1803,7 +1803,7 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>0.6563334465026855</v>
+        <v>0.1091373711824417</v>
       </c>
     </row>
     <row r="173">
@@ -1811,7 +1811,7 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>0.3625905811786652</v>
+        <v>0.0352308601140976</v>
       </c>
     </row>
     <row r="174">
@@ -1819,7 +1819,7 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>0.556209921836853</v>
+        <v>0.128654271364212</v>
       </c>
     </row>
     <row r="175">
@@ -1827,7 +1827,7 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>0.779334545135498</v>
+        <v>0.1841800957918167</v>
       </c>
     </row>
     <row r="176">
@@ -1835,7 +1835,7 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>0.6573541760444641</v>
+        <v>0.05666618794202805</v>
       </c>
     </row>
     <row r="177">
@@ -1843,7 +1843,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>0.4356926083564758</v>
+        <v>0.250083714723587</v>
       </c>
     </row>
     <row r="178">
@@ -1851,7 +1851,7 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>0.6598786115646362</v>
+        <v>0.1291818618774414</v>
       </c>
     </row>
     <row r="179">
@@ -1859,7 +1859,7 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>0.08071070164442062</v>
+        <v>0.05178101360797882</v>
       </c>
     </row>
     <row r="180">
@@ -1867,7 +1867,7 @@
         <v>178</v>
       </c>
       <c r="B180" t="n">
-        <v>0.5030912160873413</v>
+        <v>-0.01331228576600552</v>
       </c>
     </row>
     <row r="181">
@@ -1875,7 +1875,7 @@
         <v>179</v>
       </c>
       <c r="B181" t="n">
-        <v>0.3984063863754272</v>
+        <v>-0.008294121362268925</v>
       </c>
     </row>
     <row r="182">
@@ -1883,7 +1883,7 @@
         <v>180</v>
       </c>
       <c r="B182" t="n">
-        <v>0.695335865020752</v>
+        <v>0.04231686145067215</v>
       </c>
     </row>
     <row r="183">
@@ -1891,7 +1891,7 @@
         <v>181</v>
       </c>
       <c r="B183" t="n">
-        <v>0.6452840566635132</v>
+        <v>0.04145744815468788</v>
       </c>
     </row>
     <row r="184">
@@ -1899,7 +1899,7 @@
         <v>182</v>
       </c>
       <c r="B184" t="n">
-        <v>0.3681568801403046</v>
+        <v>0.1328330785036087</v>
       </c>
     </row>
     <row r="185">
@@ -1907,7 +1907,7 @@
         <v>183</v>
       </c>
       <c r="B185" t="n">
-        <v>0.6338929533958435</v>
+        <v>0.1374818384647369</v>
       </c>
     </row>
     <row r="186">
@@ -1915,7 +1915,7 @@
         <v>184</v>
       </c>
       <c r="B186" t="n">
-        <v>0.3899437785148621</v>
+        <v>-0.03955801203846931</v>
       </c>
     </row>
     <row r="187">
@@ -1923,7 +1923,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="n">
-        <v>0.4644167721271515</v>
+        <v>0.03204460814595222</v>
       </c>
     </row>
     <row r="188">
@@ -1931,7 +1931,7 @@
         <v>186</v>
       </c>
       <c r="B188" t="n">
-        <v>0.4627735316753387</v>
+        <v>0.006312794983386993</v>
       </c>
     </row>
     <row r="189">
@@ -1939,7 +1939,7 @@
         <v>187</v>
       </c>
       <c r="B189" t="n">
-        <v>0.5749266147613525</v>
+        <v>0.03430503606796265</v>
       </c>
     </row>
     <row r="190">
@@ -1947,7 +1947,7 @@
         <v>188</v>
       </c>
       <c r="B190" t="n">
-        <v>0.6312191486358643</v>
+        <v>0.1866662204265594</v>
       </c>
     </row>
     <row r="191">
@@ -1955,7 +1955,7 @@
         <v>189</v>
       </c>
       <c r="B191" t="n">
-        <v>0.5915489196777344</v>
+        <v>0.1914462447166443</v>
       </c>
     </row>
     <row r="192">
@@ -1963,7 +1963,7 @@
         <v>190</v>
       </c>
       <c r="B192" t="n">
-        <v>0.8803046345710754</v>
+        <v>0.02845238707959652</v>
       </c>
     </row>
     <row r="193">
@@ -1971,7 +1971,7 @@
         <v>191</v>
       </c>
       <c r="B193" t="n">
-        <v>0.3883032202720642</v>
+        <v>0.1920820474624634</v>
       </c>
     </row>
     <row r="194">
@@ -1979,7 +1979,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="n">
-        <v>0.6913920640945435</v>
+        <v>0.1243797764182091</v>
       </c>
     </row>
     <row r="195">
@@ -1987,7 +1987,7 @@
         <v>193</v>
       </c>
       <c r="B195" t="n">
-        <v>0.6121551990509033</v>
+        <v>0.0812239795923233</v>
       </c>
     </row>
     <row r="196">
@@ -1995,7 +1995,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="n">
-        <v>0.6827068328857422</v>
+        <v>0.08766960352659225</v>
       </c>
     </row>
     <row r="197">
@@ -2003,7 +2003,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="n">
-        <v>0.7839042544364929</v>
+        <v>0.08828277140855789</v>
       </c>
     </row>
     <row r="198">
@@ -2011,7 +2011,7 @@
         <v>196</v>
       </c>
       <c r="B198" t="n">
-        <v>0.6297519207000732</v>
+        <v>-0.07646498084068298</v>
       </c>
     </row>
     <row r="199">
@@ -2019,7 +2019,7 @@
         <v>197</v>
       </c>
       <c r="B199" t="n">
-        <v>0.5138713121414185</v>
+        <v>0.1734523326158524</v>
       </c>
     </row>
     <row r="200">
@@ -2027,7 +2027,7 @@
         <v>198</v>
       </c>
       <c r="B200" t="n">
-        <v>0.3976235389709473</v>
+        <v>0.06827311217784882</v>
       </c>
     </row>
     <row r="201">
@@ -2035,7 +2035,7 @@
         <v>199</v>
       </c>
       <c r="B201" t="n">
-        <v>0.6419792175292969</v>
+        <v>0.01178224943578243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>